<commit_message>
excel template 파일 수정
</commit_message>
<xml_diff>
--- a/src/main/resources/areaNameTestCase.xlsx
+++ b/src/main/resources/areaNameTestCase.xlsx
@@ -14,61 +14,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>xpath</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>areaName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>expectedValue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>tcNum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opt.sortsim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opt.sortdate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opt.sortfold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>opt.sortunfold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//form[@id="blog_option_sort_form"]//*[@class='clo_op']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//form[@id="blog_option_sort_form"]//button[span='정확도']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//form[@id="blog_option_sort_form"]//button[span='최신순']</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>result</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tcNum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정확도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최신순</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>접기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>열기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>opt.sortsim</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>opt.sortdate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>opt.sortfold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>opt.sortunfold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>//ul[@class="sorting"]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -413,23 +401,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.375" customWidth="1"/>
-    <col min="2" max="2" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -438,66 +425,51 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
areaname row 삭제 및 AreaTestCase, AreaTeasCasesFactory 에서 areaname 관련항목 삭제
</commit_message>
<xml_diff>
--- a/src/main/resources/areaNameTestCase.xlsx
+++ b/src/main/resources/areaNameTestCase.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18255" windowHeight="12270"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="블로그" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -404,7 +404,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>

<commit_message>
AreaNameCasesFactory 내의 testcase 수정 excel template 수정
</commit_message>
<xml_diff>
--- a/src/main/resources/areaNameTestCase.xlsx
+++ b/src/main/resources/areaNameTestCase.xlsx
@@ -44,24 +44,21 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>//form[@id="blog_option_sort_form"]//*[@class='clo_op']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>//form[@id="blog_option_sort_form"]//button[span='정확도']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>//form[@id="blog_option_sort_form"]//button[span='최신순']</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>result</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>end</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//form[@id='blog_option_sort_form']//button[span='정확도']</t>
+  </si>
+  <si>
+    <t>//form[@id='blog_option_sort_form']//button[span='최신순']</t>
+  </si>
+  <si>
+    <t>//form[@id='blog_option_sort_form']//*[@class='clo_op']</t>
   </si>
 </sst>
 </file>
@@ -408,7 +405,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -429,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -437,7 +434,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -448,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -459,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -470,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -478,7 +475,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="D6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>